<commit_message>
Changing scripts for  binding figure generation
</commit_message>
<xml_diff>
--- a/CXE24_docking/Vina/Enzyme_vs_pherobase/Enzyme_vs_pherobase-param_generator.xlsx
+++ b/CXE24_docking/Vina/Enzyme_vs_pherobase/Enzyme_vs_pherobase-param_generator.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pro\Publications_Rapports\202x-Fruitet_et_al.-CXE24\GitHub\HsubCXE24\CXE24_docking\Vina\Enzyme_vs_pherobase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A11AA93-281E-4271-A8D5-44E4E2EFD179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D02905D-76AC-4C47-86F8-052A1B82574E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0DB5A2FD-D19E-4BED-8A07-E83B80345682}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="5" r:id="rId1"/>
-    <sheet name="Script" sheetId="6" r:id="rId2"/>
+    <sheet name="backup" sheetId="7" r:id="rId2"/>
+    <sheet name="Script" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -537,11 +538,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB602B6-21F9-403C-BEAC-305D3E4E3332}">
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,27 +681,27 @@
         <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HvirCXE24_noSP_ranked0_orient.pdbqt'</v>
       </c>
       <c r="O2" s="1" t="str">
-        <f t="shared" ref="O2:O4" si="0">_xlfn.CONCAT(" --center_x ",D2)</f>
+        <f>_xlfn.CONCAT(" --center_x ",D2)</f>
         <v xml:space="preserve"> --center_x 9</v>
       </c>
       <c r="P2" s="1" t="str">
-        <f t="shared" ref="P2:P4" si="1">_xlfn.CONCAT(" --center_y ",E2)</f>
+        <f>_xlfn.CONCAT(" --center_y ",E2)</f>
         <v xml:space="preserve"> --center_y 0</v>
       </c>
       <c r="Q2" s="1" t="str">
-        <f t="shared" ref="Q2:Q4" si="2">_xlfn.CONCAT(" --center_z ",F2)</f>
+        <f>_xlfn.CONCAT(" --center_z ",F2)</f>
         <v xml:space="preserve"> --center_z 1</v>
       </c>
       <c r="R2" s="1" t="str">
-        <f t="shared" ref="R2:R4" si="3">_xlfn.CONCAT(" --size_x ",G2)</f>
+        <f>_xlfn.CONCAT(" --size_x ",G2)</f>
         <v xml:space="preserve"> --size_x 15</v>
       </c>
       <c r="S2" s="1" t="str">
-        <f t="shared" ref="S2:S4" si="4">_xlfn.CONCAT(" --size_y ",H2)</f>
+        <f>_xlfn.CONCAT(" --size_y ",H2)</f>
         <v xml:space="preserve"> --size_y 20</v>
       </c>
       <c r="T2" s="1" t="str">
-        <f t="shared" ref="T2:T4" si="5">_xlfn.CONCAT(" --size_z ",I2)</f>
+        <f>_xlfn.CONCAT(" --size_z ",I2)</f>
         <v xml:space="preserve"> --size_z 20</v>
       </c>
       <c r="U2" s="1" t="str">
@@ -758,27 +759,27 @@
         <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HvirCXE24_noSP_ranked0_orient.pdbqt'</v>
       </c>
       <c r="O3" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(" --center_x ",D3)</f>
         <v xml:space="preserve"> --center_x 9</v>
       </c>
       <c r="P3" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(" --center_y ",E3)</f>
         <v xml:space="preserve"> --center_y 0</v>
       </c>
       <c r="Q3" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(" --center_z ",F3)</f>
         <v xml:space="preserve"> --center_z 1</v>
       </c>
       <c r="R3" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f>_xlfn.CONCAT(" --size_x ",G3)</f>
         <v xml:space="preserve"> --size_x 15</v>
       </c>
       <c r="S3" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f>_xlfn.CONCAT(" --size_y ",H3)</f>
         <v xml:space="preserve"> --size_y 20</v>
       </c>
       <c r="T3" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f>_xlfn.CONCAT(" --size_z ",I3)</f>
         <v xml:space="preserve"> --size_z 20</v>
       </c>
       <c r="U3" s="1" t="str">
@@ -836,27 +837,27 @@
         <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HvirCXE24_noSP_ranked0_orient.pdbqt'</v>
       </c>
       <c r="O4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(" --center_x ",D4)</f>
         <v xml:space="preserve"> --center_x 9</v>
       </c>
       <c r="P4" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(" --center_y ",E4)</f>
         <v xml:space="preserve"> --center_y 0</v>
       </c>
       <c r="Q4" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(" --center_z ",F4)</f>
         <v xml:space="preserve"> --center_z 1</v>
       </c>
       <c r="R4" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f>_xlfn.CONCAT(" --size_x ",G4)</f>
         <v xml:space="preserve"> --size_x 15</v>
       </c>
       <c r="S4" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f>_xlfn.CONCAT(" --size_y ",H4)</f>
         <v xml:space="preserve"> --size_y 20</v>
       </c>
       <c r="T4" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f>_xlfn.CONCAT(" --size_z ",I4)</f>
         <v xml:space="preserve"> --size_z 20</v>
       </c>
       <c r="U4" s="5" t="str">
@@ -873,7 +874,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -911,30 +912,30 @@
       </c>
       <c r="N5" s="1" t="str">
         <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B5,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE5_noSP_ranked0_orient.pdbqt'</v>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_allele1_noSP_ranked0_orient.pdbqt'</v>
       </c>
       <c r="O5" s="1" t="str">
-        <f t="shared" ref="O5:O22" si="6">_xlfn.CONCAT(" --center_x ",D5)</f>
+        <f>_xlfn.CONCAT(" --center_x ",D5)</f>
         <v xml:space="preserve"> --center_x 9</v>
       </c>
       <c r="P5" s="1" t="str">
-        <f t="shared" ref="P5:P22" si="7">_xlfn.CONCAT(" --center_y ",E5)</f>
+        <f>_xlfn.CONCAT(" --center_y ",E5)</f>
         <v xml:space="preserve"> --center_y 0</v>
       </c>
       <c r="Q5" s="1" t="str">
-        <f t="shared" ref="Q5:Q22" si="8">_xlfn.CONCAT(" --center_z ",F5)</f>
+        <f>_xlfn.CONCAT(" --center_z ",F5)</f>
         <v xml:space="preserve"> --center_z 1</v>
       </c>
       <c r="R5" s="1" t="str">
-        <f t="shared" ref="R5:R22" si="9">_xlfn.CONCAT(" --size_x ",G5)</f>
+        <f>_xlfn.CONCAT(" --size_x ",G5)</f>
         <v xml:space="preserve"> --size_x 15</v>
       </c>
       <c r="S5" s="1" t="str">
-        <f t="shared" ref="S5:S22" si="10">_xlfn.CONCAT(" --size_y ",H5)</f>
+        <f>_xlfn.CONCAT(" --size_y ",H5)</f>
         <v xml:space="preserve"> --size_y 20</v>
       </c>
       <c r="T5" s="1" t="str">
-        <f t="shared" ref="T5:T22" si="11">_xlfn.CONCAT(" --size_z ",I5)</f>
+        <f>_xlfn.CONCAT(" --size_z ",I5)</f>
         <v xml:space="preserve"> --size_z 20</v>
       </c>
       <c r="U5" s="1" t="str">
@@ -943,7 +944,7 @@
       </c>
       <c r="V5" s="3" t="str">
         <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B5,"_pocket_",C5,"_vs_",K5,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE5_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_allele1_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
@@ -951,7 +952,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -989,30 +990,30 @@
       </c>
       <c r="N6" s="1" t="str">
         <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B6,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE5_noSP_ranked0_orient.pdbqt'</v>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_allele1_noSP_ranked0_orient.pdbqt'</v>
       </c>
       <c r="O6" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f>_xlfn.CONCAT(" --center_x ",D6)</f>
         <v xml:space="preserve"> --center_x 9</v>
       </c>
       <c r="P6" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT(" --center_y ",E6)</f>
         <v xml:space="preserve"> --center_y 0</v>
       </c>
       <c r="Q6" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(" --center_z ",F6)</f>
         <v xml:space="preserve"> --center_z 1</v>
       </c>
       <c r="R6" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT(" --size_x ",G6)</f>
         <v xml:space="preserve"> --size_x 15</v>
       </c>
       <c r="S6" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(" --size_y ",H6)</f>
         <v xml:space="preserve"> --size_y 20</v>
       </c>
       <c r="T6" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(" --size_z ",I6)</f>
         <v xml:space="preserve"> --size_z 20</v>
       </c>
       <c r="U6" s="1" t="str">
@@ -1021,7 +1022,7 @@
       </c>
       <c r="V6" s="3" t="str">
         <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B6,"_pocket_",C6,"_vs_",K6,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE5_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_allele1_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1029,7 +1030,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -1067,30 +1068,30 @@
       </c>
       <c r="N7" s="5" t="str">
         <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B7,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE5_noSP_ranked0_orient.pdbqt'</v>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_allele1_noSP_ranked0_orient.pdbqt'</v>
       </c>
       <c r="O7" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f>_xlfn.CONCAT(" --center_x ",D7)</f>
         <v xml:space="preserve"> --center_x 9</v>
       </c>
       <c r="P7" s="5" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT(" --center_y ",E7)</f>
         <v xml:space="preserve"> --center_y 0</v>
       </c>
       <c r="Q7" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(" --center_z ",F7)</f>
         <v xml:space="preserve"> --center_z 1</v>
       </c>
       <c r="R7" s="5" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT(" --size_x ",G7)</f>
         <v xml:space="preserve"> --size_x 15</v>
       </c>
       <c r="S7" s="5" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(" --size_y ",H7)</f>
         <v xml:space="preserve"> --size_y 20</v>
       </c>
       <c r="T7" s="5" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(" --size_z ",I7)</f>
         <v xml:space="preserve"> --size_z 20</v>
       </c>
       <c r="U7" s="5" t="str">
@@ -1099,7 +1100,7 @@
       </c>
       <c r="V7" s="3" t="str">
         <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B7,"_pocket_",C7,"_vs_",K7,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE5_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_allele1_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
@@ -1107,7 +1108,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -1145,30 +1146,30 @@
       </c>
       <c r="N8" s="1" t="str">
         <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B8,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE16_noSP_ranked0_orient.pdbqt'</v>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del28_noSP_ranked0_orient.pdbqt'</v>
       </c>
       <c r="O8" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f>_xlfn.CONCAT(" --center_x ",D8)</f>
         <v xml:space="preserve"> --center_x 9</v>
       </c>
       <c r="P8" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT(" --center_y ",E8)</f>
         <v xml:space="preserve"> --center_y 0</v>
       </c>
       <c r="Q8" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(" --center_z ",F8)</f>
         <v xml:space="preserve"> --center_z 1</v>
       </c>
       <c r="R8" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT(" --size_x ",G8)</f>
         <v xml:space="preserve"> --size_x 15</v>
       </c>
       <c r="S8" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(" --size_y ",H8)</f>
         <v xml:space="preserve"> --size_y 20</v>
       </c>
       <c r="T8" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(" --size_z ",I8)</f>
         <v xml:space="preserve"> --size_z 20</v>
       </c>
       <c r="U8" s="1" t="str">
@@ -1177,7 +1178,7 @@
       </c>
       <c r="V8" s="3" t="str">
         <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B8,"_pocket_",C8,"_vs_",K8,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE16_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del28_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
@@ -1185,7 +1186,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -1223,30 +1224,30 @@
       </c>
       <c r="N9" s="1" t="str">
         <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B9,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE16_noSP_ranked0_orient.pdbqt'</v>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del28_noSP_ranked0_orient.pdbqt'</v>
       </c>
       <c r="O9" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f>_xlfn.CONCAT(" --center_x ",D9)</f>
         <v xml:space="preserve"> --center_x 9</v>
       </c>
       <c r="P9" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT(" --center_y ",E9)</f>
         <v xml:space="preserve"> --center_y 0</v>
       </c>
       <c r="Q9" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(" --center_z ",F9)</f>
         <v xml:space="preserve"> --center_z 1</v>
       </c>
       <c r="R9" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT(" --size_x ",G9)</f>
         <v xml:space="preserve"> --size_x 15</v>
       </c>
       <c r="S9" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(" --size_y ",H9)</f>
         <v xml:space="preserve"> --size_y 20</v>
       </c>
       <c r="T9" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(" --size_z ",I9)</f>
         <v xml:space="preserve"> --size_z 20</v>
       </c>
       <c r="U9" s="1" t="str">
@@ -1255,7 +1256,7 @@
       </c>
       <c r="V9" s="3" t="str">
         <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B9,"_pocket_",C9,"_vs_",K9,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE16_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del28_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1263,7 +1264,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -1301,30 +1302,30 @@
       </c>
       <c r="N10" s="5" t="str">
         <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B10,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE16_noSP_ranked0_orient.pdbqt'</v>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del28_noSP_ranked0_orient.pdbqt'</v>
       </c>
       <c r="O10" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f>_xlfn.CONCAT(" --center_x ",D10)</f>
         <v xml:space="preserve"> --center_x 9</v>
       </c>
       <c r="P10" s="5" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT(" --center_y ",E10)</f>
         <v xml:space="preserve"> --center_y 0</v>
       </c>
       <c r="Q10" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(" --center_z ",F10)</f>
         <v xml:space="preserve"> --center_z 1</v>
       </c>
       <c r="R10" s="5" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT(" --size_x ",G10)</f>
         <v xml:space="preserve"> --size_x 15</v>
       </c>
       <c r="S10" s="5" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(" --size_y ",H10)</f>
         <v xml:space="preserve"> --size_y 20</v>
       </c>
       <c r="T10" s="5" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(" --size_z ",I10)</f>
         <v xml:space="preserve"> --size_z 20</v>
       </c>
       <c r="U10" s="5" t="str">
@@ -1333,7 +1334,7 @@
       </c>
       <c r="V10" s="3" t="str">
         <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B10,"_pocket_",C10,"_vs_",K10,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE16_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del28_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
@@ -1341,7 +1342,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -1379,30 +1380,30 @@
       </c>
       <c r="N11" s="1" t="str">
         <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B11,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_allele1_noSP_ranked0_orient.pdbqt'</v>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del31_noSP_ranked0_orient.pdbqt'</v>
       </c>
       <c r="O11" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f>_xlfn.CONCAT(" --center_x ",D11)</f>
         <v xml:space="preserve"> --center_x 9</v>
       </c>
       <c r="P11" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT(" --center_y ",E11)</f>
         <v xml:space="preserve"> --center_y 0</v>
       </c>
       <c r="Q11" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(" --center_z ",F11)</f>
         <v xml:space="preserve"> --center_z 1</v>
       </c>
       <c r="R11" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT(" --size_x ",G11)</f>
         <v xml:space="preserve"> --size_x 15</v>
       </c>
       <c r="S11" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(" --size_y ",H11)</f>
         <v xml:space="preserve"> --size_y 20</v>
       </c>
       <c r="T11" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(" --size_z ",I11)</f>
         <v xml:space="preserve"> --size_z 20</v>
       </c>
       <c r="U11" s="1" t="str">
@@ -1411,7 +1412,7 @@
       </c>
       <c r="V11" s="3" t="str">
         <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B11,"_pocket_",C11,"_vs_",K11,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_allele1_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del31_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
@@ -1419,7 +1420,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -1457,30 +1458,30 @@
       </c>
       <c r="N12" s="1" t="str">
         <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B12,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_allele1_noSP_ranked0_orient.pdbqt'</v>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del31_noSP_ranked0_orient.pdbqt'</v>
       </c>
       <c r="O12" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f>_xlfn.CONCAT(" --center_x ",D12)</f>
         <v xml:space="preserve"> --center_x 9</v>
       </c>
       <c r="P12" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT(" --center_y ",E12)</f>
         <v xml:space="preserve"> --center_y 0</v>
       </c>
       <c r="Q12" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(" --center_z ",F12)</f>
         <v xml:space="preserve"> --center_z 1</v>
       </c>
       <c r="R12" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT(" --size_x ",G12)</f>
         <v xml:space="preserve"> --size_x 15</v>
       </c>
       <c r="S12" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(" --size_y ",H12)</f>
         <v xml:space="preserve"> --size_y 20</v>
       </c>
       <c r="T12" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(" --size_z ",I12)</f>
         <v xml:space="preserve"> --size_z 20</v>
       </c>
       <c r="U12" s="1" t="str">
@@ -1489,7 +1490,7 @@
       </c>
       <c r="V12" s="3" t="str">
         <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B12,"_pocket_",C12,"_vs_",K12,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_allele1_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del31_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1497,7 +1498,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
@@ -1535,30 +1536,30 @@
       </c>
       <c r="N13" s="5" t="str">
         <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B13,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_allele1_noSP_ranked0_orient.pdbqt'</v>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del31_noSP_ranked0_orient.pdbqt'</v>
       </c>
       <c r="O13" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f>_xlfn.CONCAT(" --center_x ",D13)</f>
         <v xml:space="preserve"> --center_x 9</v>
       </c>
       <c r="P13" s="5" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT(" --center_y ",E13)</f>
         <v xml:space="preserve"> --center_y 0</v>
       </c>
       <c r="Q13" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(" --center_z ",F13)</f>
         <v xml:space="preserve"> --center_z 1</v>
       </c>
       <c r="R13" s="5" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT(" --size_x ",G13)</f>
         <v xml:space="preserve"> --size_x 15</v>
       </c>
       <c r="S13" s="5" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(" --size_y ",H13)</f>
         <v xml:space="preserve"> --size_y 20</v>
       </c>
       <c r="T13" s="5" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(" --size_z ",I13)</f>
         <v xml:space="preserve"> --size_z 20</v>
       </c>
       <c r="U13" s="5" t="str">
@@ -1567,7 +1568,7 @@
       </c>
       <c r="V13" s="3" t="str">
         <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B13,"_pocket_",C13,"_vs_",K13,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_allele1_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del31_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
@@ -1575,7 +1576,7 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -1613,30 +1614,30 @@
       </c>
       <c r="N14" s="1" t="str">
         <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B14,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del28_noSP_ranked0_orient.pdbqt'</v>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient.pdbqt'</v>
       </c>
       <c r="O14" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f>_xlfn.CONCAT(" --center_x ",D14)</f>
         <v xml:space="preserve"> --center_x 9</v>
       </c>
       <c r="P14" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT(" --center_y ",E14)</f>
         <v xml:space="preserve"> --center_y 0</v>
       </c>
       <c r="Q14" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(" --center_z ",F14)</f>
         <v xml:space="preserve"> --center_z 1</v>
       </c>
       <c r="R14" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT(" --size_x ",G14)</f>
         <v xml:space="preserve"> --size_x 15</v>
       </c>
       <c r="S14" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(" --size_y ",H14)</f>
         <v xml:space="preserve"> --size_y 20</v>
       </c>
       <c r="T14" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(" --size_z ",I14)</f>
         <v xml:space="preserve"> --size_z 20</v>
       </c>
       <c r="U14" s="1" t="str">
@@ -1645,7 +1646,7 @@
       </c>
       <c r="V14" s="3" t="str">
         <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B14,"_pocket_",C14,"_vs_",K14,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del28_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
@@ -1653,7 +1654,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -1691,30 +1692,30 @@
       </c>
       <c r="N15" s="1" t="str">
         <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B15,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del28_noSP_ranked0_orient.pdbqt'</v>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient.pdbqt'</v>
       </c>
       <c r="O15" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f>_xlfn.CONCAT(" --center_x ",D15)</f>
         <v xml:space="preserve"> --center_x 9</v>
       </c>
       <c r="P15" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT(" --center_y ",E15)</f>
         <v xml:space="preserve"> --center_y 0</v>
       </c>
       <c r="Q15" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(" --center_z ",F15)</f>
         <v xml:space="preserve"> --center_z 1</v>
       </c>
       <c r="R15" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT(" --size_x ",G15)</f>
         <v xml:space="preserve"> --size_x 15</v>
       </c>
       <c r="S15" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(" --size_y ",H15)</f>
         <v xml:space="preserve"> --size_y 20</v>
       </c>
       <c r="T15" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(" --size_z ",I15)</f>
         <v xml:space="preserve"> --size_z 20</v>
       </c>
       <c r="U15" s="1" t="str">
@@ -1723,7 +1724,7 @@
       </c>
       <c r="V15" s="3" t="str">
         <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B15,"_pocket_",C15,"_vs_",K15,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del28_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1731,7 +1732,7 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
@@ -1769,30 +1770,30 @@
       </c>
       <c r="N16" s="5" t="str">
         <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B16,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del28_noSP_ranked0_orient.pdbqt'</v>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient.pdbqt'</v>
       </c>
       <c r="O16" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f>_xlfn.CONCAT(" --center_x ",D16)</f>
         <v xml:space="preserve"> --center_x 9</v>
       </c>
       <c r="P16" s="5" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT(" --center_y ",E16)</f>
         <v xml:space="preserve"> --center_y 0</v>
       </c>
       <c r="Q16" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(" --center_z ",F16)</f>
         <v xml:space="preserve"> --center_z 1</v>
       </c>
       <c r="R16" s="5" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT(" --size_x ",G16)</f>
         <v xml:space="preserve"> --size_x 15</v>
       </c>
       <c r="S16" s="5" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(" --size_y ",H16)</f>
         <v xml:space="preserve"> --size_y 20</v>
       </c>
       <c r="T16" s="5" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(" --size_z ",I16)</f>
         <v xml:space="preserve"> --size_z 20</v>
       </c>
       <c r="U16" s="5" t="str">
@@ -1801,481 +1802,13 @@
       </c>
       <c r="V16" s="3" t="str">
         <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B16,"_pocket_",C16,"_vs_",K16,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del28_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1">
-        <v>9</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1</v>
-      </c>
-      <c r="G17" s="6">
-        <v>15</v>
-      </c>
-      <c r="H17" s="6">
-        <v>20</v>
-      </c>
-      <c r="I17" s="6">
-        <v>20</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M17" s="1" t="str">
-        <f>_xlfn.CONCAT(" --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\",A17,"-config.txt'")</f>
-        <v xml:space="preserve"> --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'</v>
-      </c>
-      <c r="N17" s="1" t="str">
-        <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B17,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del31_noSP_ranked0_orient.pdbqt'</v>
-      </c>
-      <c r="O17" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> --center_x 9</v>
-      </c>
-      <c r="P17" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve"> --center_y 0</v>
-      </c>
-      <c r="Q17" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve"> --center_z 1</v>
-      </c>
-      <c r="R17" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> --size_x 15</v>
-      </c>
-      <c r="S17" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> --size_y 20</v>
-      </c>
-      <c r="T17" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve"> --size_z 20</v>
-      </c>
-      <c r="U17" s="1" t="str">
-        <f>_xlfn.CONCAT(" --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\",J17,"\",K17,".pdbqt'")</f>
-        <v xml:space="preserve"> --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z11-16Ac.pdbqt'</v>
-      </c>
-      <c r="V17" s="3" t="str">
-        <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B17,"_pocket_",C17,"_vs_",K17,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del31_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1">
-        <v>9</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1</v>
-      </c>
-      <c r="G18" s="6">
-        <v>15</v>
-      </c>
-      <c r="H18" s="6">
-        <v>20</v>
-      </c>
-      <c r="I18" s="6">
-        <v>20</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M18" s="1" t="str">
-        <f>_xlfn.CONCAT(" --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\",A18,"-config.txt'")</f>
-        <v xml:space="preserve"> --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'</v>
-      </c>
-      <c r="N18" s="1" t="str">
-        <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B18,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del31_noSP_ranked0_orient.pdbqt'</v>
-      </c>
-      <c r="O18" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> --center_x 9</v>
-      </c>
-      <c r="P18" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve"> --center_y 0</v>
-      </c>
-      <c r="Q18" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve"> --center_z 1</v>
-      </c>
-      <c r="R18" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> --size_x 15</v>
-      </c>
-      <c r="S18" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> --size_y 20</v>
-      </c>
-      <c r="T18" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve"> --size_z 20</v>
-      </c>
-      <c r="U18" s="1" t="str">
-        <f>_xlfn.CONCAT(" --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\",J18,"\",K18,".pdbqt'")</f>
-        <v xml:space="preserve"> --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z7-16Ac.pdbqt'</v>
-      </c>
-      <c r="V18" s="3" t="str">
-        <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B18,"_pocket_",C18,"_vs_",K18,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del31_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="5">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>9</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1</v>
-      </c>
-      <c r="G19" s="6">
-        <v>15</v>
-      </c>
-      <c r="H19" s="6">
-        <v>20</v>
-      </c>
-      <c r="I19" s="6">
-        <v>20</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="M19" s="1" t="str">
-        <f>_xlfn.CONCAT(" --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\",A19,"-config.txt'")</f>
-        <v xml:space="preserve"> --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'</v>
-      </c>
-      <c r="N19" s="5" t="str">
-        <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B19,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del31_noSP_ranked0_orient.pdbqt'</v>
-      </c>
-      <c r="O19" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> --center_x 9</v>
-      </c>
-      <c r="P19" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve"> --center_y 0</v>
-      </c>
-      <c r="Q19" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve"> --center_z 1</v>
-      </c>
-      <c r="R19" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> --size_x 15</v>
-      </c>
-      <c r="S19" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> --size_y 20</v>
-      </c>
-      <c r="T19" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve"> --size_z 20</v>
-      </c>
-      <c r="U19" s="5" t="str">
-        <f>_xlfn.CONCAT(" --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\",J19,"\",K19,".pdbqt'")</f>
-        <v xml:space="preserve"> --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z9-16Ac.pdbqt'</v>
-      </c>
-      <c r="V19" s="3" t="str">
-        <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B19,"_pocket_",C19,"_vs_",K19,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del31_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1">
-        <v>9</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-      <c r="F20" s="1">
-        <v>1</v>
-      </c>
-      <c r="G20" s="6">
-        <v>15</v>
-      </c>
-      <c r="H20" s="6">
-        <v>20</v>
-      </c>
-      <c r="I20" s="6">
-        <v>20</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M20" s="1" t="str">
-        <f>_xlfn.CONCAT(" --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\",A20,"-config.txt'")</f>
-        <v xml:space="preserve"> --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'</v>
-      </c>
-      <c r="N20" s="1" t="str">
-        <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B20,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient.pdbqt'</v>
-      </c>
-      <c r="O20" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> --center_x 9</v>
-      </c>
-      <c r="P20" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve"> --center_y 0</v>
-      </c>
-      <c r="Q20" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve"> --center_z 1</v>
-      </c>
-      <c r="R20" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> --size_x 15</v>
-      </c>
-      <c r="S20" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> --size_y 20</v>
-      </c>
-      <c r="T20" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve"> --size_z 20</v>
-      </c>
-      <c r="U20" s="1" t="str">
-        <f>_xlfn.CONCAT(" --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\",J20,"\",K20,".pdbqt'")</f>
-        <v xml:space="preserve"> --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z11-16Ac.pdbqt'</v>
-      </c>
-      <c r="V20" s="3" t="str">
-        <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B20,"_pocket_",C20,"_vs_",K20,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1">
-        <v>9</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-      <c r="F21" s="1">
-        <v>1</v>
-      </c>
-      <c r="G21" s="6">
-        <v>15</v>
-      </c>
-      <c r="H21" s="6">
-        <v>20</v>
-      </c>
-      <c r="I21" s="6">
-        <v>20</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M21" s="1" t="str">
-        <f>_xlfn.CONCAT(" --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\",A21,"-config.txt'")</f>
-        <v xml:space="preserve"> --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'</v>
-      </c>
-      <c r="N21" s="1" t="str">
-        <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B21,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient.pdbqt'</v>
-      </c>
-      <c r="O21" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> --center_x 9</v>
-      </c>
-      <c r="P21" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve"> --center_y 0</v>
-      </c>
-      <c r="Q21" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve"> --center_z 1</v>
-      </c>
-      <c r="R21" s="1" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> --size_x 15</v>
-      </c>
-      <c r="S21" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> --size_y 20</v>
-      </c>
-      <c r="T21" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve"> --size_z 20</v>
-      </c>
-      <c r="U21" s="1" t="str">
-        <f>_xlfn.CONCAT(" --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\",J21,"\",K21,".pdbqt'")</f>
-        <v xml:space="preserve"> --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z7-16Ac.pdbqt'</v>
-      </c>
-      <c r="V21" s="3" t="str">
-        <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B21,"_pocket_",C21,"_vs_",K21,".pdbqt'")</f>
-        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="5">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1">
-        <v>9</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-      <c r="G22" s="6">
-        <v>15</v>
-      </c>
-      <c r="H22" s="6">
-        <v>20</v>
-      </c>
-      <c r="I22" s="6">
-        <v>20</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="M22" s="1" t="str">
-        <f>_xlfn.CONCAT(" --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\",A22,"-config.txt'")</f>
-        <v xml:space="preserve"> --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'</v>
-      </c>
-      <c r="N22" s="5" t="str">
-        <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B22,".pdbqt'")</f>
-        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient.pdbqt'</v>
-      </c>
-      <c r="O22" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> --center_x 9</v>
-      </c>
-      <c r="P22" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve"> --center_y 0</v>
-      </c>
-      <c r="Q22" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve"> --center_z 1</v>
-      </c>
-      <c r="R22" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> --size_x 15</v>
-      </c>
-      <c r="S22" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> --size_y 20</v>
-      </c>
-      <c r="T22" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve"> --size_z 20</v>
-      </c>
-      <c r="U22" s="5" t="str">
-        <f>_xlfn.CONCAT(" --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\",J22,"\",K22,".pdbqt'")</f>
-        <v xml:space="preserve"> --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z9-16Ac.pdbqt'</v>
-      </c>
-      <c r="V22" s="3" t="str">
-        <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B22,"_pocket_",C22,"_vs_",K22,".pdbqt'")</f>
         <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V13">
-    <sortCondition ref="B2:B13"/>
-    <sortCondition ref="K2:K13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V7">
+    <sortCondition ref="B2:B7"/>
+    <sortCondition ref="K2:K7"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2283,6 +1816,489 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF794F1C-E752-40BA-9BEF-F70FDBAFD954}">
+  <dimension ref="A1:V6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1" s="6">
+        <v>15</v>
+      </c>
+      <c r="H1" s="6">
+        <v>20</v>
+      </c>
+      <c r="I1" s="6">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="1" t="str">
+        <f>_xlfn.CONCAT(" --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\",A1,"-config.txt'")</f>
+        <v xml:space="preserve"> --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'</v>
+      </c>
+      <c r="N1" s="1" t="str">
+        <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B1,".pdbqt'")</f>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE5_noSP_ranked0_orient.pdbqt'</v>
+      </c>
+      <c r="O1" s="1" t="str">
+        <f>_xlfn.CONCAT(" --center_x ",D1)</f>
+        <v xml:space="preserve"> --center_x 9</v>
+      </c>
+      <c r="P1" s="1" t="str">
+        <f>_xlfn.CONCAT(" --center_y ",E1)</f>
+        <v xml:space="preserve"> --center_y 0</v>
+      </c>
+      <c r="Q1" s="1" t="str">
+        <f>_xlfn.CONCAT(" --center_z ",F1)</f>
+        <v xml:space="preserve"> --center_z 1</v>
+      </c>
+      <c r="R1" s="1" t="str">
+        <f>_xlfn.CONCAT(" --size_x ",G1)</f>
+        <v xml:space="preserve"> --size_x 15</v>
+      </c>
+      <c r="S1" s="1" t="str">
+        <f>_xlfn.CONCAT(" --size_y ",H1)</f>
+        <v xml:space="preserve"> --size_y 20</v>
+      </c>
+      <c r="T1" s="1" t="str">
+        <f>_xlfn.CONCAT(" --size_z ",I1)</f>
+        <v xml:space="preserve"> --size_z 20</v>
+      </c>
+      <c r="U1" s="1" t="str">
+        <f>_xlfn.CONCAT(" --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\",J1,"\",K1,".pdbqt'")</f>
+        <v xml:space="preserve"> --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z11-16Ac.pdbqt'</v>
+      </c>
+      <c r="V1" s="3" t="str">
+        <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B1,"_pocket_",C1,"_vs_",K1,".pdbqt'")</f>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE5_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>15</v>
+      </c>
+      <c r="H2" s="6">
+        <v>20</v>
+      </c>
+      <c r="I2" s="6">
+        <v>20</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="str">
+        <f>_xlfn.CONCAT(" --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\",A2,"-config.txt'")</f>
+        <v xml:space="preserve"> --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'</v>
+      </c>
+      <c r="N2" s="1" t="str">
+        <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B2,".pdbqt'")</f>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE5_noSP_ranked0_orient.pdbqt'</v>
+      </c>
+      <c r="O2" s="1" t="str">
+        <f>_xlfn.CONCAT(" --center_x ",D2)</f>
+        <v xml:space="preserve"> --center_x 9</v>
+      </c>
+      <c r="P2" s="1" t="str">
+        <f>_xlfn.CONCAT(" --center_y ",E2)</f>
+        <v xml:space="preserve"> --center_y 0</v>
+      </c>
+      <c r="Q2" s="1" t="str">
+        <f>_xlfn.CONCAT(" --center_z ",F2)</f>
+        <v xml:space="preserve"> --center_z 1</v>
+      </c>
+      <c r="R2" s="1" t="str">
+        <f>_xlfn.CONCAT(" --size_x ",G2)</f>
+        <v xml:space="preserve"> --size_x 15</v>
+      </c>
+      <c r="S2" s="1" t="str">
+        <f>_xlfn.CONCAT(" --size_y ",H2)</f>
+        <v xml:space="preserve"> --size_y 20</v>
+      </c>
+      <c r="T2" s="1" t="str">
+        <f>_xlfn.CONCAT(" --size_z ",I2)</f>
+        <v xml:space="preserve"> --size_z 20</v>
+      </c>
+      <c r="U2" s="1" t="str">
+        <f>_xlfn.CONCAT(" --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\",J2,"\",K2,".pdbqt'")</f>
+        <v xml:space="preserve"> --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z7-16Ac.pdbqt'</v>
+      </c>
+      <c r="V2" s="3" t="str">
+        <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B2,"_pocket_",C2,"_vs_",K2,".pdbqt'")</f>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE5_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6">
+        <v>15</v>
+      </c>
+      <c r="H3" s="6">
+        <v>20</v>
+      </c>
+      <c r="I3" s="6">
+        <v>20</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1" t="str">
+        <f>_xlfn.CONCAT(" --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\",A3,"-config.txt'")</f>
+        <v xml:space="preserve"> --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'</v>
+      </c>
+      <c r="N3" s="5" t="str">
+        <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B3,".pdbqt'")</f>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE5_noSP_ranked0_orient.pdbqt'</v>
+      </c>
+      <c r="O3" s="5" t="str">
+        <f>_xlfn.CONCAT(" --center_x ",D3)</f>
+        <v xml:space="preserve"> --center_x 9</v>
+      </c>
+      <c r="P3" s="5" t="str">
+        <f>_xlfn.CONCAT(" --center_y ",E3)</f>
+        <v xml:space="preserve"> --center_y 0</v>
+      </c>
+      <c r="Q3" s="5" t="str">
+        <f>_xlfn.CONCAT(" --center_z ",F3)</f>
+        <v xml:space="preserve"> --center_z 1</v>
+      </c>
+      <c r="R3" s="5" t="str">
+        <f>_xlfn.CONCAT(" --size_x ",G3)</f>
+        <v xml:space="preserve"> --size_x 15</v>
+      </c>
+      <c r="S3" s="5" t="str">
+        <f>_xlfn.CONCAT(" --size_y ",H3)</f>
+        <v xml:space="preserve"> --size_y 20</v>
+      </c>
+      <c r="T3" s="5" t="str">
+        <f>_xlfn.CONCAT(" --size_z ",I3)</f>
+        <v xml:space="preserve"> --size_z 20</v>
+      </c>
+      <c r="U3" s="5" t="str">
+        <f>_xlfn.CONCAT(" --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\",J3,"\",K3,".pdbqt'")</f>
+        <v xml:space="preserve"> --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z9-16Ac.pdbqt'</v>
+      </c>
+      <c r="V3" s="3" t="str">
+        <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B3,"_pocket_",C3,"_vs_",K3,".pdbqt'")</f>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE5_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>15</v>
+      </c>
+      <c r="H4" s="6">
+        <v>20</v>
+      </c>
+      <c r="I4" s="6">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1" t="str">
+        <f>_xlfn.CONCAT(" --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\",A4,"-config.txt'")</f>
+        <v xml:space="preserve"> --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'</v>
+      </c>
+      <c r="N4" s="1" t="str">
+        <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B4,".pdbqt'")</f>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE16_noSP_ranked0_orient.pdbqt'</v>
+      </c>
+      <c r="O4" s="1" t="str">
+        <f>_xlfn.CONCAT(" --center_x ",D4)</f>
+        <v xml:space="preserve"> --center_x 9</v>
+      </c>
+      <c r="P4" s="1" t="str">
+        <f>_xlfn.CONCAT(" --center_y ",E4)</f>
+        <v xml:space="preserve"> --center_y 0</v>
+      </c>
+      <c r="Q4" s="1" t="str">
+        <f>_xlfn.CONCAT(" --center_z ",F4)</f>
+        <v xml:space="preserve"> --center_z 1</v>
+      </c>
+      <c r="R4" s="1" t="str">
+        <f>_xlfn.CONCAT(" --size_x ",G4)</f>
+        <v xml:space="preserve"> --size_x 15</v>
+      </c>
+      <c r="S4" s="1" t="str">
+        <f>_xlfn.CONCAT(" --size_y ",H4)</f>
+        <v xml:space="preserve"> --size_y 20</v>
+      </c>
+      <c r="T4" s="1" t="str">
+        <f>_xlfn.CONCAT(" --size_z ",I4)</f>
+        <v xml:space="preserve"> --size_z 20</v>
+      </c>
+      <c r="U4" s="1" t="str">
+        <f>_xlfn.CONCAT(" --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\",J4,"\",K4,".pdbqt'")</f>
+        <v xml:space="preserve"> --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z11-16Ac.pdbqt'</v>
+      </c>
+      <c r="V4" s="3" t="str">
+        <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B4,"_pocket_",C4,"_vs_",K4,".pdbqt'")</f>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE16_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6">
+        <v>15</v>
+      </c>
+      <c r="H5" s="6">
+        <v>20</v>
+      </c>
+      <c r="I5" s="6">
+        <v>20</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1" t="str">
+        <f>_xlfn.CONCAT(" --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\",A5,"-config.txt'")</f>
+        <v xml:space="preserve"> --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'</v>
+      </c>
+      <c r="N5" s="1" t="str">
+        <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B5,".pdbqt'")</f>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE16_noSP_ranked0_orient.pdbqt'</v>
+      </c>
+      <c r="O5" s="1" t="str">
+        <f>_xlfn.CONCAT(" --center_x ",D5)</f>
+        <v xml:space="preserve"> --center_x 9</v>
+      </c>
+      <c r="P5" s="1" t="str">
+        <f>_xlfn.CONCAT(" --center_y ",E5)</f>
+        <v xml:space="preserve"> --center_y 0</v>
+      </c>
+      <c r="Q5" s="1" t="str">
+        <f>_xlfn.CONCAT(" --center_z ",F5)</f>
+        <v xml:space="preserve"> --center_z 1</v>
+      </c>
+      <c r="R5" s="1" t="str">
+        <f>_xlfn.CONCAT(" --size_x ",G5)</f>
+        <v xml:space="preserve"> --size_x 15</v>
+      </c>
+      <c r="S5" s="1" t="str">
+        <f>_xlfn.CONCAT(" --size_y ",H5)</f>
+        <v xml:space="preserve"> --size_y 20</v>
+      </c>
+      <c r="T5" s="1" t="str">
+        <f>_xlfn.CONCAT(" --size_z ",I5)</f>
+        <v xml:space="preserve"> --size_z 20</v>
+      </c>
+      <c r="U5" s="1" t="str">
+        <f>_xlfn.CONCAT(" --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\",J5,"\",K5,".pdbqt'")</f>
+        <v xml:space="preserve"> --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z7-16Ac.pdbqt'</v>
+      </c>
+      <c r="V5" s="3" t="str">
+        <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B5,"_pocket_",C5,"_vs_",K5,".pdbqt'")</f>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE16_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6">
+        <v>15</v>
+      </c>
+      <c r="H6" s="6">
+        <v>20</v>
+      </c>
+      <c r="I6" s="6">
+        <v>20</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1" t="str">
+        <f>_xlfn.CONCAT(" --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\",A6,"-config.txt'")</f>
+        <v xml:space="preserve"> --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'</v>
+      </c>
+      <c r="N6" s="5" t="str">
+        <f>_xlfn.CONCAT(" --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\",B6,".pdbqt'")</f>
+        <v xml:space="preserve"> --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE16_noSP_ranked0_orient.pdbqt'</v>
+      </c>
+      <c r="O6" s="5" t="str">
+        <f>_xlfn.CONCAT(" --center_x ",D6)</f>
+        <v xml:space="preserve"> --center_x 9</v>
+      </c>
+      <c r="P6" s="5" t="str">
+        <f>_xlfn.CONCAT(" --center_y ",E6)</f>
+        <v xml:space="preserve"> --center_y 0</v>
+      </c>
+      <c r="Q6" s="5" t="str">
+        <f>_xlfn.CONCAT(" --center_z ",F6)</f>
+        <v xml:space="preserve"> --center_z 1</v>
+      </c>
+      <c r="R6" s="5" t="str">
+        <f>_xlfn.CONCAT(" --size_x ",G6)</f>
+        <v xml:space="preserve"> --size_x 15</v>
+      </c>
+      <c r="S6" s="5" t="str">
+        <f>_xlfn.CONCAT(" --size_y ",H6)</f>
+        <v xml:space="preserve"> --size_y 20</v>
+      </c>
+      <c r="T6" s="5" t="str">
+        <f>_xlfn.CONCAT(" --size_z ",I6)</f>
+        <v xml:space="preserve"> --size_z 20</v>
+      </c>
+      <c r="U6" s="5" t="str">
+        <f>_xlfn.CONCAT(" --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\",J6,"\",K6,".pdbqt'")</f>
+        <v xml:space="preserve"> --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z9-16Ac.pdbqt'</v>
+      </c>
+      <c r="V6" s="3" t="str">
+        <f>_xlfn.CONCAT(" --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\",B6,"_pocket_",C6,"_vs_",K6,".pdbqt'")</f>
+        <v xml:space="preserve"> --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE16_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B9E72E-FAB0-461E-8EA8-E54F4FC7CDC4}">
   <dimension ref="A1:A48"/>
   <sheetViews>
@@ -2312,109 +2328,109 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
-        <f>_xlfn.CONCAT(variables!L5," ",variables!M5," ",variables!N5," ",variables!O5," ",variables!P5," ",variables!Q5," ",variables!R5," ",variables!S5," ",variables!T5," ",variables!U5," ",variables!V5)</f>
+        <f>_xlfn.CONCAT(backup!L1," ",backup!M1," ",backup!N1," ",backup!O1," ",backup!P1," ",backup!Q1," ",backup!R1," ",backup!S1," ",backup!T1," ",backup!U1," ",backup!V1)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE5_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z11-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE5_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
-        <f>_xlfn.CONCAT(variables!L6," ",variables!M6," ",variables!N6," ",variables!O6," ",variables!P6," ",variables!Q6," ",variables!R6," ",variables!S6," ",variables!T6," ",variables!U6," ",variables!V6)</f>
+        <f>_xlfn.CONCAT(backup!L2," ",backup!M2," ",backup!N2," ",backup!O2," ",backup!P2," ",backup!Q2," ",backup!R2," ",backup!S2," ",backup!T2," ",backup!U2," ",backup!V2)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE5_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z7-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE5_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
-        <f>_xlfn.CONCAT(variables!L7," ",variables!M7," ",variables!N7," ",variables!O7," ",variables!P7," ",variables!Q7," ",variables!R7," ",variables!S7," ",variables!T7," ",variables!U7," ",variables!V7)</f>
+        <f>_xlfn.CONCAT(backup!L3," ",backup!M3," ",backup!N3," ",backup!O3," ",backup!P3," ",backup!Q3," ",backup!R3," ",backup!S3," ",backup!T3," ",backup!U3," ",backup!V3)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE5_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z9-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE5_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
-        <f>_xlfn.CONCAT(variables!L8," ",variables!M8," ",variables!N8," ",variables!O8," ",variables!P8," ",variables!Q8," ",variables!R8," ",variables!S8," ",variables!T8," ",variables!U8," ",variables!V8)</f>
+        <f>_xlfn.CONCAT(backup!L4," ",backup!M4," ",backup!N4," ",backup!O4," ",backup!P4," ",backup!Q4," ",backup!R4," ",backup!S4," ",backup!T4," ",backup!U4," ",backup!V4)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE16_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z11-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE16_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
-        <f>_xlfn.CONCAT(variables!L9," ",variables!M9," ",variables!N9," ",variables!O9," ",variables!P9," ",variables!Q9," ",variables!R9," ",variables!S9," ",variables!T9," ",variables!U9," ",variables!V9)</f>
+        <f>_xlfn.CONCAT(backup!L5," ",backup!M5," ",backup!N5," ",backup!O5," ",backup!P5," ",backup!Q5," ",backup!R5," ",backup!S5," ",backup!T5," ",backup!U5," ",backup!V5)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE16_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z7-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE16_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
-        <f>_xlfn.CONCAT(variables!L10," ",variables!M10," ",variables!N10," ",variables!O10," ",variables!P10," ",variables!Q10," ",variables!R10," ",variables!S10," ",variables!T10," ",variables!U10," ",variables!V10)</f>
+        <f>_xlfn.CONCAT(backup!L6," ",backup!M6," ",backup!N6," ",backup!O6," ",backup!P6," ",backup!Q6," ",backup!R6," ",backup!S6," ",backup!T6," ",backup!U6," ",backup!V6)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE16_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z9-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE16_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
-        <f>_xlfn.CONCAT(variables!L11," ",variables!M11," ",variables!N11," ",variables!O11," ",variables!P11," ",variables!Q11," ",variables!R11," ",variables!S11," ",variables!T11," ",variables!U11," ",variables!V11)</f>
+        <f>_xlfn.CONCAT(variables!L5," ",variables!M5," ",variables!N5," ",variables!O5," ",variables!P5," ",variables!Q5," ",variables!R5," ",variables!S5," ",variables!T5," ",variables!U5," ",variables!V5)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_allele1_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z11-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_allele1_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
-        <f>_xlfn.CONCAT(variables!L12," ",variables!M12," ",variables!N12," ",variables!O12," ",variables!P12," ",variables!Q12," ",variables!R12," ",variables!S12," ",variables!T12," ",variables!U12," ",variables!V12)</f>
+        <f>_xlfn.CONCAT(variables!L6," ",variables!M6," ",variables!N6," ",variables!O6," ",variables!P6," ",variables!Q6," ",variables!R6," ",variables!S6," ",variables!T6," ",variables!U6," ",variables!V6)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_allele1_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z7-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_allele1_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
-        <f>_xlfn.CONCAT(variables!L13," ",variables!M13," ",variables!N13," ",variables!O13," ",variables!P13," ",variables!Q13," ",variables!R13," ",variables!S13," ",variables!T13," ",variables!U13," ",variables!V13)</f>
+        <f>_xlfn.CONCAT(variables!L7," ",variables!M7," ",variables!N7," ",variables!O7," ",variables!P7," ",variables!Q7," ",variables!R7," ",variables!S7," ",variables!T7," ",variables!U7," ",variables!V7)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_allele1_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z9-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_allele1_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
-        <f>_xlfn.CONCAT(variables!L14," ",variables!M14," ",variables!N14," ",variables!O14," ",variables!P14," ",variables!Q14," ",variables!R14," ",variables!S14," ",variables!T14," ",variables!U14," ",variables!V14)</f>
+        <f>_xlfn.CONCAT(variables!L8," ",variables!M8," ",variables!N8," ",variables!O8," ",variables!P8," ",variables!Q8," ",variables!R8," ",variables!S8," ",variables!T8," ",variables!U8," ",variables!V8)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del28_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z11-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del28_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
-        <f>_xlfn.CONCAT(variables!L15," ",variables!M15," ",variables!N15," ",variables!O15," ",variables!P15," ",variables!Q15," ",variables!R15," ",variables!S15," ",variables!T15," ",variables!U15," ",variables!V15)</f>
+        <f>_xlfn.CONCAT(variables!L9," ",variables!M9," ",variables!N9," ",variables!O9," ",variables!P9," ",variables!Q9," ",variables!R9," ",variables!S9," ",variables!T9," ",variables!U9," ",variables!V9)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del28_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z7-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del28_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
-        <f>_xlfn.CONCAT(variables!L16," ",variables!M16," ",variables!N16," ",variables!O16," ",variables!P16," ",variables!Q16," ",variables!R16," ",variables!S16," ",variables!T16," ",variables!U16," ",variables!V16)</f>
+        <f>_xlfn.CONCAT(variables!L10," ",variables!M10," ",variables!N10," ",variables!O10," ",variables!P10," ",variables!Q10," ",variables!R10," ",variables!S10," ",variables!T10," ",variables!U10," ",variables!V10)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del28_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z9-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del28_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
-        <f>_xlfn.CONCAT(variables!L17," ",variables!M17," ",variables!N17," ",variables!O17," ",variables!P17," ",variables!Q17," ",variables!R17," ",variables!S17," ",variables!T17," ",variables!U17," ",variables!V17)</f>
+        <f>_xlfn.CONCAT(variables!L11," ",variables!M11," ",variables!N11," ",variables!O11," ",variables!P11," ",variables!Q11," ",variables!R11," ",variables!S11," ",variables!T11," ",variables!U11," ",variables!V11)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del31_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z11-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del31_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
-        <f>_xlfn.CONCAT(variables!L18," ",variables!M18," ",variables!N18," ",variables!O18," ",variables!P18," ",variables!Q18," ",variables!R18," ",variables!S18," ",variables!T18," ",variables!U18," ",variables!V18)</f>
+        <f>_xlfn.CONCAT(variables!L12," ",variables!M12," ",variables!N12," ",variables!O12," ",variables!P12," ",variables!Q12," ",variables!R12," ",variables!S12," ",variables!T12," ",variables!U12," ",variables!V12)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del31_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z7-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del31_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
-        <f>_xlfn.CONCAT(variables!L19," ",variables!M19," ",variables!N19," ",variables!O19," ",variables!P19," ",variables!Q19," ",variables!R19," ",variables!S19," ",variables!T19," ",variables!U19," ",variables!V19)</f>
+        <f>_xlfn.CONCAT(variables!L13," ",variables!M13," ",variables!N13," ",variables!O13," ",variables!P13," ",variables!Q13," ",variables!R13," ",variables!S13," ",variables!T13," ",variables!U13," ",variables!V13)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_del31_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z9-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_del31_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
-        <f>_xlfn.CONCAT(variables!L20," ",variables!M20," ",variables!N20," ",variables!O20," ",variables!P20," ",variables!Q20," ",variables!R20," ",variables!S20," ",variables!T20," ",variables!U20," ",variables!V20)</f>
+        <f>_xlfn.CONCAT(variables!L14," ",variables!M14," ",variables!N14," ",variables!O14," ",variables!P14," ",variables!Q14," ",variables!R14," ",variables!S14," ",variables!T14," ",variables!U14," ",variables!V14)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z11-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient_pocket_1_vs_Z11-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
-        <f>_xlfn.CONCAT(variables!L21," ",variables!M21," ",variables!N21," ",variables!O21," ",variables!P21," ",variables!Q21," ",variables!R21," ",variables!S21," ",variables!T21," ",variables!U21," ",variables!V21)</f>
+        <f>_xlfn.CONCAT(variables!L15," ",variables!M15," ",variables!N15," ",variables!O15," ",variables!P15," ",variables!Q15," ",variables!R15," ",variables!S15," ",variables!T15," ",variables!U15," ",variables!V15)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z7-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient_pocket_1_vs_Z7-16Ac.pdbqt'</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
-        <f>_xlfn.CONCAT(variables!L22," ",variables!M22," ",variables!N22," ",variables!O22," ",variables!P22," ",variables!Q22," ",variables!R22," ",variables!S22," ",variables!T22," ",variables!U22," ",variables!V22)</f>
+        <f>_xlfn.CONCAT(variables!L16," ",variables!M16," ",variables!N16," ",variables!O16," ",variables!P16," ",variables!Q16," ",variables!R16," ",variables!S16," ",variables!T16," ",variables!U16," ",variables!V16)</f>
         <v>C:\Pro\Programmes\Vina\vina_1.2.3_windows_x86_64.exe  --config 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\Enzyme_vs_pherobase-config.txt'  --receptor 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient.pdbqt'  --center_x 9  --center_y 0  --center_z 1  --size_x 15  --size_y 20  --size_z 20  --ligand 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Autodocktools\Z9-16Ac.pdbqt'  --out 'C:\Pro\Projets\Heliothis Acetate production\CXE24_docking\Vina\Enzyme_vs_pherobase\output\HsubCXE24_HsubTED_trunc_noSP_ranked0_orient_pocket_1_vs_Z9-16Ac.pdbqt'</v>
       </c>
     </row>
@@ -2438,145 +2454,145 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
+        <f>_xlfn.CONCAT(variables!L17," ",variables!M17," ",variables!N17," ",variables!O17," ",variables!P17," ",variables!Q17," ",variables!R17," ",variables!S17," ",variables!T17," ",variables!U17," ",variables!V17)</f>
+        <v xml:space="preserve">          </v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <f>_xlfn.CONCAT(variables!L18," ",variables!M18," ",variables!N18," ",variables!O18," ",variables!P18," ",variables!Q18," ",variables!R18," ",variables!S18," ",variables!T18," ",variables!U18," ",variables!V18)</f>
+        <v xml:space="preserve">          </v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <f>_xlfn.CONCAT(variables!L19," ",variables!M19," ",variables!N19," ",variables!O19," ",variables!P19," ",variables!Q19," ",variables!R19," ",variables!S19," ",variables!T19," ",variables!U19," ",variables!V19)</f>
+        <v xml:space="preserve">          </v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <f>_xlfn.CONCAT(variables!L20," ",variables!M20," ",variables!N20," ",variables!O20," ",variables!P20," ",variables!Q20," ",variables!R20," ",variables!S20," ",variables!T20," ",variables!U20," ",variables!V20)</f>
+        <v xml:space="preserve">          </v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
+        <f>_xlfn.CONCAT(variables!L21," ",variables!M21," ",variables!N21," ",variables!O21," ",variables!P21," ",variables!Q21," ",variables!R21," ",variables!S21," ",variables!T21," ",variables!U21," ",variables!V21)</f>
+        <v xml:space="preserve">          </v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
+        <f>_xlfn.CONCAT(variables!L22," ",variables!M22," ",variables!N22," ",variables!O22," ",variables!P22," ",variables!Q22," ",variables!R22," ",variables!S22," ",variables!T22," ",variables!U22," ",variables!V22)</f>
+        <v xml:space="preserve">          </v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
         <f>_xlfn.CONCAT(variables!L23," ",variables!M23," ",variables!N23," ",variables!O23," ",variables!P23," ",variables!Q23," ",variables!R23," ",variables!S23," ",variables!T23," ",variables!U23," ",variables!V23)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="str">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
         <f>_xlfn.CONCAT(variables!L24," ",variables!M24," ",variables!N24," ",variables!O24," ",variables!P24," ",variables!Q24," ",variables!R24," ",variables!S24," ",variables!T24," ",variables!U24," ",variables!V24)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="str">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
         <f>_xlfn.CONCAT(variables!L25," ",variables!M25," ",variables!N25," ",variables!O25," ",variables!P25," ",variables!Q25," ",variables!R25," ",variables!S25," ",variables!T25," ",variables!U25," ",variables!V25)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="str">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
         <f>_xlfn.CONCAT(variables!L26," ",variables!M26," ",variables!N26," ",variables!O26," ",variables!P26," ",variables!Q26," ",variables!R26," ",variables!S26," ",variables!T26," ",variables!U26," ",variables!V26)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="str">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
         <f>_xlfn.CONCAT(variables!L27," ",variables!M27," ",variables!N27," ",variables!O27," ",variables!P27," ",variables!Q27," ",variables!R27," ",variables!S27," ",variables!T27," ",variables!U27," ",variables!V27)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="str">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
         <f>_xlfn.CONCAT(variables!L28," ",variables!M28," ",variables!N28," ",variables!O28," ",variables!P28," ",variables!Q28," ",variables!R28," ",variables!S28," ",variables!T28," ",variables!U28," ",variables!V28)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="str">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="str">
         <f>_xlfn.CONCAT(variables!L29," ",variables!M29," ",variables!N29," ",variables!O29," ",variables!P29," ",variables!Q29," ",variables!R29," ",variables!S29," ",variables!T29," ",variables!U29," ",variables!V29)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="str">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="str">
         <f>_xlfn.CONCAT(variables!L30," ",variables!M30," ",variables!N30," ",variables!O30," ",variables!P30," ",variables!Q30," ",variables!R30," ",variables!S30," ",variables!T30," ",variables!U30," ",variables!V30)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="str">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="str">
         <f>_xlfn.CONCAT(variables!L31," ",variables!M31," ",variables!N31," ",variables!O31," ",variables!P31," ",variables!Q31," ",variables!R31," ",variables!S31," ",variables!T31," ",variables!U31," ",variables!V31)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="str">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="str">
         <f>_xlfn.CONCAT(variables!L32," ",variables!M32," ",variables!N32," ",variables!O32," ",variables!P32," ",variables!Q32," ",variables!R32," ",variables!S32," ",variables!T32," ",variables!U32," ",variables!V32)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="str">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="str">
         <f>_xlfn.CONCAT(variables!L33," ",variables!M33," ",variables!N33," ",variables!O33," ",variables!P33," ",variables!Q33," ",variables!R33," ",variables!S33," ",variables!T33," ",variables!U33," ",variables!V33)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="str">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="str">
         <f>_xlfn.CONCAT(variables!L34," ",variables!M34," ",variables!N34," ",variables!O34," ",variables!P34," ",variables!Q34," ",variables!R34," ",variables!S34," ",variables!T34," ",variables!U34," ",variables!V34)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="str">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="str">
         <f>_xlfn.CONCAT(variables!L35," ",variables!M35," ",variables!N35," ",variables!O35," ",variables!P35," ",variables!Q35," ",variables!R35," ",variables!S35," ",variables!T35," ",variables!U35," ",variables!V35)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="str">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="str">
         <f>_xlfn.CONCAT(variables!L36," ",variables!M36," ",variables!N36," ",variables!O36," ",variables!P36," ",variables!Q36," ",variables!R36," ",variables!S36," ",variables!T36," ",variables!U36," ",variables!V36)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="str">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="str">
         <f>_xlfn.CONCAT(variables!L37," ",variables!M37," ",variables!N37," ",variables!O37," ",variables!P37," ",variables!Q37," ",variables!R37," ",variables!S37," ",variables!T37," ",variables!U37," ",variables!V37)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="str">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="str">
         <f>_xlfn.CONCAT(variables!L38," ",variables!M38," ",variables!N38," ",variables!O38," ",variables!P38," ",variables!Q38," ",variables!R38," ",variables!S38," ",variables!T38," ",variables!U38," ",variables!V38)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="str">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="str">
         <f>_xlfn.CONCAT(variables!L39," ",variables!M39," ",variables!N39," ",variables!O39," ",variables!P39," ",variables!Q39," ",variables!R39," ",variables!S39," ",variables!T39," ",variables!U39," ",variables!V39)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="str">
-        <f>_xlfn.CONCAT(variables!L40," ",variables!M40," ",variables!N40," ",variables!O40," ",variables!P40," ",variables!Q40," ",variables!R40," ",variables!S40," ",variables!T40," ",variables!U40," ",variables!V40)</f>
-        <v xml:space="preserve">          </v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="str">
-        <f>_xlfn.CONCAT(variables!L41," ",variables!M41," ",variables!N41," ",variables!O41," ",variables!P41," ",variables!Q41," ",variables!R41," ",variables!S41," ",variables!T41," ",variables!U41," ",variables!V41)</f>
-        <v xml:space="preserve">          </v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="str">
-        <f>_xlfn.CONCAT(variables!L42," ",variables!M42," ",variables!N42," ",variables!O42," ",variables!P42," ",variables!Q42," ",variables!R42," ",variables!S42," ",variables!T42," ",variables!U42," ",variables!V42)</f>
-        <v xml:space="preserve">          </v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" t="str">
-        <f>_xlfn.CONCAT(variables!L43," ",variables!M43," ",variables!N43," ",variables!O43," ",variables!P43," ",variables!Q43," ",variables!R43," ",variables!S43," ",variables!T43," ",variables!U43," ",variables!V43)</f>
-        <v xml:space="preserve">          </v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="str">
-        <f>_xlfn.CONCAT(variables!L44," ",variables!M44," ",variables!N44," ",variables!O44," ",variables!P44," ",variables!Q44," ",variables!R44," ",variables!S44," ",variables!T44," ",variables!U44," ",variables!V44)</f>
-        <v xml:space="preserve">          </v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="str">
-        <f>_xlfn.CONCAT(variables!L45," ",variables!M45," ",variables!N45," ",variables!O45," ",variables!P45," ",variables!Q45," ",variables!R45," ",variables!S45," ",variables!T45," ",variables!U45," ",variables!V45)</f>
-        <v xml:space="preserve">          </v>
-      </c>
-    </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
-        <f>_xlfn.CONCAT(variables!L46," ",variables!M46," ",variables!N46," ",variables!O46," ",variables!P46," ",variables!Q46," ",variables!R46," ",variables!S46," ",variables!T46," ",variables!U46," ",variables!V46)</f>
+        <f>_xlfn.CONCAT(variables!L40," ",variables!M40," ",variables!N40," ",variables!O40," ",variables!P40," ",variables!Q40," ",variables!R40," ",variables!S40," ",variables!T40," ",variables!U40," ",variables!V40)</f>
         <v xml:space="preserve">          </v>
       </c>
     </row>

</xml_diff>